<commit_message>
GA Breakers is kind of well working
</commit_message>
<xml_diff>
--- a/pysgrs/resources/media/breaker_ga.xlsx
+++ b/pysgrs/resources/media/breaker_ga.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,17 +465,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-2545.665264706972</v>
+        <v>-2515.687903442344</v>
       </c>
       <c r="C2" t="n">
-        <v>-2375.768185353663</v>
+        <v>-2378.540182647377</v>
       </c>
       <c r="D2" t="n">
-        <v>-2209.51381355913</v>
+        <v>-2233.91874289191</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MLPBFVGTXOWVTHGVRVJQJHBPOVIEZ</t>
+          <t>RIMEKVGACZOAZALMRVWCOMUCRZWNMGISVQUV</t>
         </is>
       </c>
     </row>
@@ -484,17 +484,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-2466.046388322208</v>
+        <v>-2444.749512578723</v>
       </c>
       <c r="C3" t="n">
-        <v>-2342.690261104902</v>
+        <v>-2345.617137280339</v>
       </c>
       <c r="D3" t="n">
-        <v>-2183.12424054208</v>
+        <v>-2233.91874289191</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BLCDTUMOWZORTRYUEHRMTWAGFECHF</t>
+          <t>RIMEKVGACZOAZALMRVWCOMUCRZWNMGISVQUV</t>
         </is>
       </c>
     </row>
@@ -503,17 +503,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-2434.780914804393</v>
+        <v>-2419.127614892365</v>
       </c>
       <c r="C4" t="n">
-        <v>-2313.195201669495</v>
+        <v>-2317.674869717826</v>
       </c>
       <c r="D4" t="n">
-        <v>-2169.865805445038</v>
+        <v>-2197.751876357477</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BLCDTUMOWZORTREKHJKMKSTQZTIAV</t>
+          <t>KBTETAZHZLEEIVNMMWNCJLNFNITVVXXSVVYX</t>
         </is>
       </c>
     </row>
@@ -522,17 +522,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-2391.399695191852</v>
+        <v>-2405.03459111583</v>
       </c>
       <c r="C5" t="n">
-        <v>-2285.589816781585</v>
+        <v>-2294.948417384423</v>
       </c>
       <c r="D5" t="n">
-        <v>-2157.792851424118</v>
+        <v>-2140.5993113284</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BLCDTUMOWZURTNBOIQBTEYVZKVVEZ</t>
+          <t>EFNGUHTEOVZJSTSONHGPYCXGXZCICBOBVNLC</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-2450.500879362715</v>
+        <v>-2371.602990276165</v>
       </c>
       <c r="C6" t="n">
-        <v>-2258.446606358004</v>
+        <v>-2273.573617736322</v>
       </c>
       <c r="D6" t="n">
-        <v>-2132.706207671112</v>
+        <v>-2127.187252260248</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>BLCDTUMOWZORTRYUEHRMTWAGQVWRN</t>
+          <t>KBTETAZHZLEEIVNMMWNCJLNFNITVVXUBVUMV</t>
         </is>
       </c>
     </row>
@@ -560,17 +560,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-2331.34088107647</v>
+        <v>-2355.873999497381</v>
       </c>
       <c r="C7" t="n">
-        <v>-2234.756404996267</v>
+        <v>-2248.118188500081</v>
       </c>
       <c r="D7" t="n">
-        <v>-2098.109397085625</v>
+        <v>-2127.187252260248</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>BLCDTUMOWZORTRYUEHRMTWTGQVWRM</t>
+          <t>KBTETAZHZLEEIVNMMWNCJLNFNITVVXUBVUMV</t>
         </is>
       </c>
     </row>
@@ -579,17 +579,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-2343.13435345343</v>
+        <v>-2329.661488092737</v>
       </c>
       <c r="C8" t="n">
-        <v>-2208.725694677533</v>
+        <v>-2226.652565602505</v>
       </c>
       <c r="D8" t="n">
-        <v>-2091.289783039933</v>
+        <v>-2127.187252260248</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>BLCDTUMOWZORTRYOIQBTEYASAIURB</t>
+          <t>KBTETAZHZLEEIVNMMWNCJLNFNITVVXUBVUMV</t>
         </is>
       </c>
     </row>
@@ -598,17 +598,17 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-2309.518450775591</v>
+        <v>-2293.447633414059</v>
       </c>
       <c r="C9" t="n">
-        <v>-2182.719887590665</v>
+        <v>-2206.979505822307</v>
       </c>
       <c r="D9" t="n">
-        <v>-2063.738545792488</v>
+        <v>-2099.121510662305</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>FLCATUPVXVONEUOURUSTGLUGKNXXL</t>
+          <t>SURNPIPUURORIWGSTYMFFAUKEFCAZRUAUIMD</t>
         </is>
       </c>
     </row>
@@ -617,17 +617,17 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2280.554721442302</v>
+        <v>-2290.216820099364</v>
       </c>
       <c r="C10" t="n">
-        <v>-2161.532711024297</v>
+        <v>-2188.827512105452</v>
       </c>
       <c r="D10" t="n">
-        <v>-2039.773726575122</v>
+        <v>-2064.199398563801</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>FLJDTUMPLZORTRYOIQBTEJASAIURB</t>
+          <t>DAALLICTOTOEIVNMMWNCJLNFNITRRJMXLXLS</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-2271.561803283624</v>
+        <v>-2266.799092543843</v>
       </c>
       <c r="C11" t="n">
-        <v>-2137.218275491286</v>
+        <v>-2168.346513299218</v>
       </c>
       <c r="D11" t="n">
-        <v>-2025.257144174994</v>
+        <v>-2035.668695055668</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PLCJTUMONUFWEJRIUYGMQSRFOTEXV</t>
+          <t>GIMEKVGANZOEIVNMMWNCJXUSDIICPCUBZWRL</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-2222.821074043566</v>
+        <v>-2282.110949361741</v>
       </c>
       <c r="C12" t="n">
-        <v>-2114.726013021617</v>
+        <v>-2146.439539840875</v>
       </c>
       <c r="D12" t="n">
-        <v>-1994.506051938091</v>
+        <v>-2029.790378516839</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>PPWDTVGTXVONEJHATUZTEXTGQVATL</t>
+          <t>RUNGUHCRWGOVEZHLUJNHHUVYXTPDZRNILNMK</t>
         </is>
       </c>
     </row>
@@ -674,17 +674,17 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-2223.178327919743</v>
+        <v>-2253.224554474264</v>
       </c>
       <c r="C13" t="n">
-        <v>-2095.657939784531</v>
+        <v>-2127.910180509602</v>
       </c>
       <c r="D13" t="n">
-        <v>-1957.925894406215</v>
+        <v>-2020.885816051097</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>BLCATUPVXVONERVUTUVTUCUCKVATL</t>
+          <t>GEUKHHCRZLEEIVNMMWNCJLNFNITDRXXTAWMS</t>
         </is>
       </c>
     </row>
@@ -693,17 +693,17 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-2192.38740939039</v>
+        <v>-2222.191023958027</v>
       </c>
       <c r="C14" t="n">
-        <v>-2076.550579225348</v>
+        <v>-2107.992799578324</v>
       </c>
       <c r="D14" t="n">
-        <v>-1957.925894406215</v>
+        <v>-1985.828092587658</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>BLCATUPVXVONERVUTUVTUCUCKVATL</t>
+          <t>GEUKHHCRZLEEIALMRAWCOMUCRRIXCNOBVUMS</t>
         </is>
       </c>
     </row>
@@ -712,17 +712,17 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-2183.380381736042</v>
+        <v>-2200.002093655697</v>
       </c>
       <c r="C15" t="n">
-        <v>-2057.089970336925</v>
+        <v>-2083.510765745175</v>
       </c>
       <c r="D15" t="n">
-        <v>-1925.958944776979</v>
+        <v>-1977.951163084196</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>BLJDTUMJEIAMARGUTQZTESWSBVNPB</t>
+          <t>GITETOCNVHYDVVHOOGORORXGXZCICBOBVUMO</t>
         </is>
       </c>
     </row>
@@ -731,17 +731,17 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-2190.097996495506</v>
+        <v>-2152.942847453141</v>
       </c>
       <c r="C16" t="n">
-        <v>-2033.87547718038</v>
+        <v>-2062.881711582745</v>
       </c>
       <c r="D16" t="n">
-        <v>-1910.534523240273</v>
+        <v>-1969.243187890465</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>PDWCTUMVXEQYQRGUTQZTESWSORLSL</t>
+          <t>RIMEKRCRWRORIWGSTYMCOYLENFMXCNOBVUMS</t>
         </is>
       </c>
     </row>
@@ -750,17 +750,17 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-2142.459966122056</v>
+        <v>-2144.245078122364</v>
       </c>
       <c r="C17" t="n">
-        <v>-2012.520505677423</v>
+        <v>-2040.900928393216</v>
       </c>
       <c r="D17" t="n">
-        <v>-1879.08017577596</v>
+        <v>-1916.755973161637</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>FLUYBULJEVONERVVTUGTNTTGORWRL</t>
+          <t>GUKADENPWGOENTYMRZNCOLNFNITDRBOBLXMS</t>
         </is>
       </c>
     </row>
@@ -769,17 +769,17 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-2136.485678021094</v>
+        <v>-2152.716157260226</v>
       </c>
       <c r="C18" t="n">
-        <v>-1989.834460951723</v>
+        <v>-2023.066515929988</v>
       </c>
       <c r="D18" t="n">
-        <v>-1866.52756174059</v>
+        <v>-1872.41583489503</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>FLUDTUEVNEQYQRTVZUVTQCUCKRATL</t>
+          <t>GIMAVICTGGDEKQZMMWNCJLVENITAZNOBVUMS</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-2095.227632715256</v>
+        <v>-2116.473704782852</v>
       </c>
       <c r="C19" t="n">
-        <v>-1968.741742768104</v>
+        <v>-2003.458938474303</v>
       </c>
       <c r="D19" t="n">
-        <v>-1795.456594295276</v>
+        <v>-1863.591767043034</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>FLCATUMTXOCMARGUTQZTESWSBVAUL</t>
+          <t>EENRTAYAWGDEKQZMMWNCJLVENITAZNOBVUMS</t>
         </is>
       </c>
     </row>
@@ -807,17 +807,17 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-2101.971919105004</v>
+        <v>-2098.999098757225</v>
       </c>
       <c r="C20" t="n">
-        <v>-1941.526714395322</v>
+        <v>-1984.72004926758</v>
       </c>
       <c r="D20" t="n">
-        <v>-1782.686715084028</v>
+        <v>-1863.591767043034</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>FLUJTUEVNEQYERQBDURTEPERBVAXL</t>
+          <t>EENRTAYAWGDEKQZMMWNCJLVENITAZNOBVUMS</t>
         </is>
       </c>
     </row>
@@ -826,17 +826,17 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-2064.571314487908</v>
+        <v>-2079.049192698945</v>
       </c>
       <c r="C21" t="n">
-        <v>-1920.03433461408</v>
+        <v>-1967.958978617201</v>
       </c>
       <c r="D21" t="n">
-        <v>-1735.429862175949</v>
+        <v>-1834.021487236669</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>FLNDTUMJEICMERVVTURTEZEXORIVL</t>
+          <t>GITETOCNVUOAKQZMMWNCJLVENITAZNOBVUMS</t>
         </is>
       </c>
     </row>
@@ -845,17 +845,17 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-2039.895489186692</v>
+        <v>-2077.302109572133</v>
       </c>
       <c r="C22" t="n">
-        <v>-1893.380900046958</v>
+        <v>-1944.356265348652</v>
       </c>
       <c r="D22" t="n">
-        <v>-1700.291104318487</v>
+        <v>-1834.021487236669</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>FLNDTUMJEICMERVVTURTEZEXORATL</t>
+          <t>GITETOCNVUOAKQZMMWNCJLVENITAZNOBVUMS</t>
         </is>
       </c>
     </row>
@@ -864,17 +864,17 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-1991.270235861245</v>
+        <v>-2051.947191339192</v>
       </c>
       <c r="C23" t="n">
-        <v>-1871.358788134473</v>
+        <v>-1925.563347045025</v>
       </c>
       <c r="D23" t="n">
-        <v>-1671.293255482228</v>
+        <v>-1789.253718001349</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>FLUYTUGCNUCMERVVTURTEZEXORATL</t>
+          <t>GEUETOCALGOENVNMMWNCJLNENIICPBOBVNMS</t>
         </is>
       </c>
     </row>
@@ -883,17 +883,17 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-1985.374611798791</v>
+        <v>-2027.175122162399</v>
       </c>
       <c r="C24" t="n">
-        <v>-1842.23811208999</v>
+        <v>-1904.867628086421</v>
       </c>
       <c r="D24" t="n">
-        <v>-1671.293255482228</v>
+        <v>-1776.821369859174</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>FLUYTUGCNUCMERVVTURTEZEXORATL</t>
+          <t>GEUETOCALGOENVNMMWNCJLNENIICPBOBVUMS</t>
         </is>
       </c>
     </row>
@@ -902,17 +902,17 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-2038.801915742179</v>
+        <v>-2012.003965074844</v>
       </c>
       <c r="C25" t="n">
-        <v>-1820.66736731453</v>
+        <v>-1885.155416888669</v>
       </c>
       <c r="D25" t="n">
-        <v>-1671.293255482228</v>
+        <v>-1771.788852480876</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>FLUYTUGCNUCMERVVTURTEZEXORATL</t>
+          <t>GEUETOCALZOEIVNMMWNCGXVENICICFOBVUMS</t>
         </is>
       </c>
     </row>
@@ -921,17 +921,17 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-1960.352434180767</v>
+        <v>-2003.718576287438</v>
       </c>
       <c r="C26" t="n">
-        <v>-1797.849588307885</v>
+        <v>-1865.039734108038</v>
       </c>
       <c r="D26" t="n">
-        <v>-1668.874369300844</v>
+        <v>-1735.31137271126</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>FLUATUEVNICMERMVTUFTESUFBVWLL</t>
+          <t>GEUETOCALGOENVNMMWNCMLVENITAZTOBLEGS</t>
         </is>
       </c>
     </row>
@@ -940,17 +940,17 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-1937.738903744692</v>
+        <v>-1999.988810225627</v>
       </c>
       <c r="C27" t="n">
-        <v>-1777.120242441814</v>
+        <v>-1843.531474647455</v>
       </c>
       <c r="D27" t="n">
-        <v>-1666.342983201209</v>
+        <v>-1681.073936292828</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>FLUJTULCNECNERGUTURTESUFOEATL</t>
+          <t>GEUETICTZLERITHMMWNCOLVENIYACGOBVUMS</t>
         </is>
       </c>
     </row>
@@ -959,17 +959,17 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-1886.783840146007</v>
+        <v>-1966.820551705446</v>
       </c>
       <c r="C28" t="n">
-        <v>-1757.076110553737</v>
+        <v>-1822.369053440683</v>
       </c>
       <c r="D28" t="n">
-        <v>-1652.331000620111</v>
+        <v>-1651.990553716601</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>FLUDTUEVNECMERGUTQCTESWSBVWLL</t>
+          <t>GEXETICTZLERITHMMWNCOLVENIYNCNOBLNMS</t>
         </is>
       </c>
     </row>
@@ -978,17 +978,17 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-1888.438397505313</v>
+        <v>-1934.857555868027</v>
       </c>
       <c r="C29" t="n">
-        <v>-1735.413273279977</v>
+        <v>-1800.14302329202</v>
       </c>
       <c r="D29" t="n">
-        <v>-1605.072892818718</v>
+        <v>-1642.73123423328</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>FLUDTUEVNECMERGVTURTEPEXORAXL</t>
+          <t>GEUETICTZLERITHMMWNCOLVENIMAPCUBVEMS</t>
         </is>
       </c>
     </row>
@@ -997,17 +997,17 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-1832.059870018099</v>
+        <v>-1932.322016491481</v>
       </c>
       <c r="C30" t="n">
-        <v>-1714.138760750288</v>
+        <v>-1781.255267561023</v>
       </c>
       <c r="D30" t="n">
-        <v>-1561.402661951467</v>
+        <v>-1624.867305095261</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>FLUQTUATNUCMERVVTURTESTQKVAOL</t>
+          <t>GEXETICTZLERITHMMWNCOLVEXICICBOBVEMS</t>
         </is>
       </c>
     </row>
@@ -1016,17 +1016,17 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-1849.6062871371</v>
+        <v>-1880.021985766563</v>
       </c>
       <c r="C31" t="n">
-        <v>-1699.600786126658</v>
+        <v>-1760.708881000591</v>
       </c>
       <c r="D31" t="n">
-        <v>-1561.402661951467</v>
+        <v>-1624.867305095261</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>FLUQTUATNUCMERVVTURTESTQKVAOL</t>
+          <t>GEXETICTZLERITHMMWNCOLVEXICICBOBVEMS</t>
         </is>
       </c>
     </row>
@@ -1035,17 +1035,17 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-1808.457589127673</v>
+        <v>-1873.832931160797</v>
       </c>
       <c r="C32" t="n">
-        <v>-1681.803762766132</v>
+        <v>-1738.722424697274</v>
       </c>
       <c r="D32" t="n">
-        <v>-1561.402661951467</v>
+        <v>-1611.570651767258</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>FLUQTUATNUCMERVVTURTESTQKVAOL</t>
+          <t>GITETOCOLJORITHMMWNCOLVENICAZROBVUMS</t>
         </is>
       </c>
     </row>
@@ -1054,17 +1054,17 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-1804.387098030272</v>
+        <v>-1849.572755354076</v>
       </c>
       <c r="C33" t="n">
-        <v>-1666.393748708779</v>
+        <v>-1718.647597367039</v>
       </c>
       <c r="D33" t="n">
-        <v>-1532.662094522096</v>
+        <v>-1600.466664441236</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>FLUQTUATNUCMERVVTURTESTXORATL</t>
+          <t>GERETICTZLERITHMMAWCOLVENICAZROBLXMS</t>
         </is>
       </c>
     </row>
@@ -1073,17 +1073,17 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-1840.204512413638</v>
+        <v>-1830.425497278115</v>
       </c>
       <c r="C34" t="n">
-        <v>-1649.558240688952</v>
+        <v>-1696.375605741427</v>
       </c>
       <c r="D34" t="n">
-        <v>-1520.194128370213</v>
+        <v>-1551.57760371119</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>FLUITUEJNECMERGBTURTESJFORATL</t>
+          <t>GENETICALGERITHMMWNCULVENICICFOBVOMS</t>
         </is>
       </c>
     </row>
@@ -1092,17 +1092,17 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-1811.88371110711</v>
+        <v>-1867.551231125186</v>
       </c>
       <c r="C35" t="n">
-        <v>-1631.141739821171</v>
+        <v>-1671.691642514827</v>
       </c>
       <c r="D35" t="n">
-        <v>-1495.618869433162</v>
+        <v>-1510.505552090652</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>FLUQTUATNUCMERVVTURTESTBORAEL</t>
+          <t>GENETICALGERITHMMWNAOLIENICICBOBVEMS</t>
         </is>
       </c>
     </row>
@@ -1111,17 +1111,17 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-1774.580252112289</v>
+        <v>-1803.597879379844</v>
       </c>
       <c r="C36" t="n">
-        <v>-1614.638774924233</v>
+        <v>-1651.344726561033</v>
       </c>
       <c r="D36" t="n">
-        <v>-1495.618869433162</v>
+        <v>-1510.505552090652</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>FLUQTUATNUCMERVVTURTESTBORAEL</t>
+          <t>GENETICALGERITHMMWNAOLIENICICBOBVEMS</t>
         </is>
       </c>
     </row>
@@ -1130,17 +1130,17 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-1754.283120197577</v>
+        <v>-1777.708170289369</v>
       </c>
       <c r="C37" t="n">
-        <v>-1597.292285367132</v>
+        <v>-1634.578158306608</v>
       </c>
       <c r="D37" t="n">
-        <v>-1495.618869433162</v>
+        <v>-1462.519671668418</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>FLUQTUATNUCMERVVTURTESTBORAEL</t>
+          <t>GENETICALGEXITHMMWNCOLVENICAZROBLXMS</t>
         </is>
       </c>
     </row>
@@ -1149,17 +1149,17 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-1747.349967527418</v>
+        <v>-1761.854020488858</v>
       </c>
       <c r="C38" t="n">
-        <v>-1580.584091811681</v>
+        <v>-1611.409532756433</v>
       </c>
       <c r="D38" t="n">
-        <v>-1429.877961426985</v>
+        <v>-1425.897270793657</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>FLUCTUPTNECMERGVTURTESTXORALL</t>
+          <t>GENETICALGERITHMMWNCOLVENICAZROBVEMS</t>
         </is>
       </c>
     </row>
@@ -1168,17 +1168,17 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-1706.479717258148</v>
+        <v>-1809.170430056217</v>
       </c>
       <c r="C39" t="n">
-        <v>-1561.353874921144</v>
+        <v>-1589.58874361133</v>
       </c>
       <c r="D39" t="n">
-        <v>-1429.877961426985</v>
+        <v>-1425.897270793657</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>FLUCTUPTNECMERGVTURTESTXORALL</t>
+          <t>GENETICALGERITHMMWNCOLVENICAZROBVEMS</t>
         </is>
       </c>
     </row>
@@ -1187,17 +1187,17 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-1712.614971437168</v>
+        <v>-1693.035251121859</v>
       </c>
       <c r="C40" t="n">
-        <v>-1545.692651174216</v>
+        <v>-1572.06032899211</v>
       </c>
       <c r="D40" t="n">
-        <v>-1429.877961426985</v>
+        <v>-1406.275216550857</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>FLUCTUPTNECMERGVTURTESTXORALL</t>
+          <t>GENETICALGERITHMMANCOLVENICAZROBVEMS</t>
         </is>
       </c>
     </row>
@@ -1206,17 +1206,17 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-1680.615947487541</v>
+        <v>-1709.002733652663</v>
       </c>
       <c r="C41" t="n">
-        <v>-1528.063063888936</v>
+        <v>-1548.217688972795</v>
       </c>
       <c r="D41" t="n">
-        <v>-1424.237487186097</v>
+        <v>-1406.275216550857</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>FLUQTUATNECMERGQTURTESDFORALL</t>
+          <t>GENETICALGERITHMMANCOLVENICAZROBVEMS</t>
         </is>
       </c>
     </row>
@@ -1225,17 +1225,17 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-1710.718202724692</v>
+        <v>-1688.167836420496</v>
       </c>
       <c r="C42" t="n">
-        <v>-1514.627907169066</v>
+        <v>-1524.224738774409</v>
       </c>
       <c r="D42" t="n">
-        <v>-1413.66938197809</v>
+        <v>-1406.275216550857</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>FLUCTUPTNECMERGETURTESTFORWLL</t>
+          <t>GENETICALGERITHMMANCOLVENICAZROBVEMS</t>
         </is>
       </c>
     </row>
@@ -1244,17 +1244,17 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-1692.984153057459</v>
+        <v>-1656.68741101359</v>
       </c>
       <c r="C43" t="n">
-        <v>-1498.029760948914</v>
+        <v>-1505.319341340316</v>
       </c>
       <c r="D43" t="n">
-        <v>-1375.980412109771</v>
+        <v>-1406.275216550857</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>FLUDTUATNECMERGIDURTESTFORALL</t>
+          <t>GENETICALGERITHMMANCOLVENICAZROBVEMS</t>
         </is>
       </c>
     </row>
@@ -1263,17 +1263,17 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-1644.563797382987</v>
+        <v>-1635.614613157862</v>
       </c>
       <c r="C44" t="n">
-        <v>-1483.961937232879</v>
+        <v>-1482.866009781279</v>
       </c>
       <c r="D44" t="n">
-        <v>-1375.980412109771</v>
+        <v>-1406.275216550857</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>FLUDTUATNECMERGIDURTESTFORALL</t>
+          <t>GENETICALGERITHMMANCOLVENICAZROBVEMS</t>
         </is>
       </c>
     </row>
@@ -1282,17 +1282,17 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-1644.704229065213</v>
+        <v>-1604.474013824728</v>
       </c>
       <c r="C45" t="n">
-        <v>-1466.770327743605</v>
+        <v>-1462.519671668418</v>
       </c>
       <c r="D45" t="n">
-        <v>-1330.011801815623</v>
+        <v>-1393.250956086203</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>FLUCTUATNECMERGITURTESJFORALL</t>
+          <t>GENETICALGORITHMMWNCOLVENICAZROBLEMS</t>
         </is>
       </c>
     </row>
@@ -1301,17 +1301,17 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-1628.902491371844</v>
+        <v>-1556.884196558117</v>
       </c>
       <c r="C46" t="n">
-        <v>-1452.313368089554</v>
+        <v>-1444.90408025275</v>
       </c>
       <c r="D46" t="n">
-        <v>-1330.011801815623</v>
+        <v>-1389.267764436849</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>FLUCTUATNECMERGITURTESJFORALL</t>
+          <t>GENETICALGERITHMMANCOLVENICAZROBLEMS</t>
         </is>
       </c>
     </row>
@@ -1320,17 +1320,17 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-1593.208516624874</v>
+        <v>-1543.302300164627</v>
       </c>
       <c r="C47" t="n">
-        <v>-1436.643788303212</v>
+        <v>-1441.657591840179</v>
       </c>
       <c r="D47" t="n">
-        <v>-1330.011801815623</v>
+        <v>-1356.355923880278</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>FLUCTUATNECMERGITURTESJFORALL</t>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
         </is>
       </c>
     </row>
@@ -1339,17 +1339,17 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-1575.904047899687</v>
+        <v>-1554.102605107388</v>
       </c>
       <c r="C48" t="n">
-        <v>-1422.78296691275</v>
+        <v>-1425.897270793657</v>
       </c>
       <c r="D48" t="n">
-        <v>-1317.095766058383</v>
+        <v>-1356.355923880278</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>FLUCTUATNOCMERGITURTESTFORALL</t>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
         </is>
       </c>
     </row>
@@ -1358,17 +1358,17 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-1553.205243276431</v>
+        <v>-1561.813596369303</v>
       </c>
       <c r="C49" t="n">
-        <v>-1409.231982135181</v>
+        <v>-1424.909612613019</v>
       </c>
       <c r="D49" t="n">
-        <v>-1295.405153208076</v>
+        <v>-1356.355923880278</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>FLUCTUATNECMERGITURTESTFORALL</t>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
         </is>
       </c>
     </row>
@@ -1377,17 +1377,17 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-1551.970588762547</v>
+        <v>-1523.619244494638</v>
       </c>
       <c r="C50" t="n">
-        <v>-1393.509524402643</v>
+        <v>-1408.889818679649</v>
       </c>
       <c r="D50" t="n">
-        <v>-1295.405153208076</v>
+        <v>-1356.355923880278</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>FLUCTUATNECMERGITURTESTFORALL</t>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
         </is>
       </c>
     </row>
@@ -1396,17 +1396,967 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-1542.465571022069</v>
+        <v>-1513.055455248857</v>
       </c>
       <c r="C51" t="n">
-        <v>-1381.563157919698</v>
+        <v>-1408.889818679649</v>
       </c>
       <c r="D51" t="n">
-        <v>-1295.405153208076</v>
+        <v>-1356.355923880278</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>FLUCTUATNECMERGITURTESTFORALL</t>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>-1526.117090932946</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-1407.902160499011</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>-1539.034285389235</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-1393.250956086203</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>-1500.936915039855</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-1389.267764436849</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>-1509.109638818938</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-1389.267764436849</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>-1505.421139284573</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-1375.977978123077</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>-1510.484133666786</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-1373.628901843404</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>-1488.729509838179</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-1371.994786473723</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMMANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>-1475.530723269714</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-1365.852197981029</v>
+      </c>
+      <c r="D59" t="n">
+        <v>-1348.236606565361</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>GENETICALGERITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>-1453.554583390728</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-1348.236606565361</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>GENETICALGERITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>-1461.899562912661</v>
+      </c>
+      <c r="C61" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>-1462.914756696957</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>-1483.105868863454</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D63" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>-1461.609329537463</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>-1472.882773873808</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D65" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>-1450.905175580821</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D66" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>-1462.082126929515</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-1356.355923880278</v>
+      </c>
+      <c r="D67" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>-1472.509298728001</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-1349.870721935041</v>
+      </c>
+      <c r="D68" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>-1448.751118819639</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D69" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-1452.439618354004</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D70" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>-1438.323947021152</v>
+      </c>
+      <c r="C71" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D71" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>-1452.439618354004</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D72" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>-1433.10691927964</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D73" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-1430.97579819851</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D74" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-1452.439618354004</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D75" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>-1438.323947021152</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D76" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-1451.337384274989</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D77" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>-1438.323947021152</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D78" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-1438.323947021152</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D79" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>-1433.056138622059</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D80" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-1439.0213994628</v>
+      </c>
+      <c r="C81" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D81" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>-1452.439618354004</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D82" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>-1434.411771650226</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D83" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>-1452.439618354004</v>
+      </c>
+      <c r="C84" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D84" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-1446.758754388928</v>
+      </c>
+      <c r="C85" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D85" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>-1443.098682736346</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D86" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>-1448.751118819639</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D87" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>-1448.751118819639</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D88" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>-1434.411771650226</v>
+      </c>
+      <c r="C89" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D89" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>-1443.098682736346</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D90" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>-1449.124593965446</v>
+      </c>
+      <c r="C91" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D91" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>-1437.819361530436</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D92" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>-1436.133680767905</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D93" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>-1449.124593965446</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D94" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>-1438.879321936921</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D95" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>-1438.141383004298</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D96" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>-1440.208256068927</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D97" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-1440.208256068927</v>
+      </c>
+      <c r="C98" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D98" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-1434.350403404579</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D99" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-1439.0213994628</v>
+      </c>
+      <c r="C100" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D100" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-1436.927611776049</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="D101" t="n">
+        <v>-1332.597743971915</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>GENETICALGORITHMCANCOLVENICEZROBLEMS</t>
         </is>
       </c>
     </row>

</xml_diff>